<commit_message>
Se modificaron script de BD
Se agregó script de inserción de provincias.
Se agregó script de inserción de partidos. (A modificar por errores)
Se modificaron excel para creación de inserts masivamente.
</commit_message>
<xml_diff>
--- a/# Desarrollo BD/INSERT datos 13/05_DATOS_ref_direccion_provincia_INSERT_SUM-Provincias.xlsx
+++ b/# Desarrollo BD/INSERT datos 13/05_DATOS_ref_direccion_provincia_INSERT_SUM-Provincias.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>ID País</t>
   </si>
@@ -37,84 +37,54 @@
     <t>Buenos Aires</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>CAT</t>
   </si>
   <si>
     <t>Catamarca</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>CBA</t>
   </si>
   <si>
     <t>Córdoba</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>CFE</t>
   </si>
   <si>
     <t>Capital Federal</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>CHA</t>
   </si>
   <si>
     <t>Chaco</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>CHU</t>
   </si>
   <si>
     <t>Chubut</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>COR</t>
   </si>
   <si>
     <t>Corrientes</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>ERI</t>
   </si>
   <si>
     <t>Entre Ríos</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>FOR</t>
   </si>
   <si>
     <t>Formosa</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>FUE</t>
-  </si>
-  <si>
     <t>Desconocido</t>
   </si>
   <si>
@@ -124,133 +94,91 @@
     <t>Jujuy</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>LPA</t>
   </si>
   <si>
     <t>La Pampa</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>LRI</t>
   </si>
   <si>
     <t>La Rioja</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>MEN</t>
   </si>
   <si>
     <t>Mendoza</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>MIS</t>
   </si>
   <si>
     <t>Misiones</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
     <t>NEU</t>
   </si>
   <si>
     <t>Neuquén</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>RNE</t>
   </si>
   <si>
     <t>Río Negro</t>
   </si>
   <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>SAL</t>
   </si>
   <si>
     <t>Salta</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>SCR</t>
   </si>
   <si>
     <t>Santa Cruz</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>SDE</t>
   </si>
   <si>
     <t>Santiago del Estero</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>SFE</t>
   </si>
   <si>
     <t>Santa Fe</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>SJU</t>
   </si>
   <si>
     <t>San Juan</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>SLU</t>
   </si>
   <si>
     <t>San Luis</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>TDF</t>
   </si>
   <si>
     <t>Tierra del Fuego</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>TUC</t>
   </si>
   <si>
     <t>Tucumán</t>
   </si>
   <si>
-    <t>14</t>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -743,9 +671,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1083,9 +1012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1117,8 +1046,8 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="str">
-        <f>"INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', "</f>
-        <v xml:space="preserve">INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', </v>
+        <f>"INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), "</f>
+        <v xml:space="preserve">INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), </v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1126,17 +1055,18 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"00"</f>
+        <v>00</v>
       </c>
       <c r="E2" t="str">
-        <f>$E$1&amp;"'"&amp;$B2&amp;"', '"&amp;$C2&amp;"')"</f>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'BAI', 'Buenos Aires')</v>
+        <f>$E$1&amp;"'"&amp;$B2&amp;"', '"&amp;$C2&amp;"');"</f>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'CFE', 'Capital Federal');</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1144,17 +1074,18 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>"01"</f>
+        <v>01</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E26" si="0">$E$1&amp;"'"&amp;$B3&amp;"', '"&amp;$C3&amp;"')"</f>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'CAT', 'Catamarca')</v>
+        <f t="shared" ref="E3:E26" si="0">$E$1&amp;"'"&amp;$B3&amp;"', '"&amp;$C3&amp;"');"</f>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'BAI', 'Buenos Aires');</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1162,17 +1093,18 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>"02"</f>
+        <v>02</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'CBA', 'Córdoba')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'CAT', 'Catamarca');</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1180,17 +1112,18 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>"03"</f>
+        <v>03</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'CFE', 'Capital Federal')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'CBA', 'Córdoba');</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1203,12 +1136,13 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
+      <c r="D6" s="2" t="str">
+        <f>"04"</f>
+        <v>04</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'CHA', 'Chaco')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'COR', 'Corrientes');</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1216,17 +1150,18 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
+      <c r="D7" s="2" t="str">
+        <f>"05"</f>
+        <v>05</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'CHU', 'Chubut')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'ERI', 'Entre Ríos');</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1234,17 +1169,18 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
         <v>25</v>
       </c>
+      <c r="D8" s="2" t="str">
+        <f>"06"</f>
+        <v>06</v>
+      </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'COR', 'Corrientes')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'JUJ', 'Jujuy');</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1252,17 +1188,18 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>"07"</f>
+        <v>07</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'ERI', 'Entre Ríos')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'MEN', 'Mendoza');</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1270,17 +1207,18 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
+      <c r="D10" s="2" t="str">
+        <f>"08"</f>
+        <v>08</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'FOR', 'Formosa')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'LRI', 'La Rioja');</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1288,14 +1226,18 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>"09"</f>
+        <v>09</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'FUE', 'Desconocido')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'SAL', 'Salta');</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1303,17 +1245,18 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>"10"</f>
+        <v>10</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'JUJ', 'Jujuy')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'SJU', 'San Juan');</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1321,17 +1264,18 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
+        <v>49</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>"11"</f>
+        <v>11</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'LPA', 'La Pampa')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'SLU', 'San Luis');</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1339,17 +1283,18 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>"12"</f>
+        <v>12</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'LRI', 'La Rioja')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'SFE', 'Santa Fe');</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1357,17 +1302,18 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
+      <c r="D15" s="2" t="str">
+        <f>"13"</f>
+        <v>13</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'MEN', 'Mendoza')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'SDE', 'Santiago del Estero');</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1375,17 +1321,18 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
+        <v>53</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>"14"</f>
+        <v>14</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'MIS', 'Misiones')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'TUC', 'Tucumán');</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1393,17 +1340,18 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>51</v>
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>"16"</f>
+        <v>16</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'NEU', 'Neuquén')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'CHA', 'Chaco');</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1411,17 +1359,18 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" t="s">
-        <v>54</v>
+        <v>16</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f>"17"</f>
+        <v>17</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'RNE', 'Río Negro')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'CHU', 'Chubut');</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1429,17 +1378,18 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>57</v>
+        <v>22</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f>"18"</f>
+        <v>18</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'SAL', 'Salta')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'FOR', 'Formosa');</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1447,17 +1397,18 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
+        <v>33</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f>"19"</f>
+        <v>19</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'SCR', 'Santa Cruz')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'MIS', 'Misiones');</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1465,17 +1416,18 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" t="s">
-        <v>63</v>
+        <v>35</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f>"20"</f>
+        <v>20</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'SDE', 'Santiago del Estero')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'NEU', 'Neuquén');</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1483,17 +1435,18 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" t="s">
-        <v>66</v>
+        <v>27</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f>"21"</f>
+        <v>21</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'SFE', 'Santa Fe')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'LPA', 'La Pampa');</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1501,17 +1454,18 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>69</v>
+        <v>37</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f>"22"</f>
+        <v>22</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'SJU', 'San Juan')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'RNE', 'Río Negro');</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1519,17 +1473,18 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" t="s">
-        <v>72</v>
+        <v>41</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f>"23"</f>
+        <v>23</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'SLU', 'San Luis')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'SCR', 'Santa Cruz');</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1537,17 +1492,18 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" t="s">
-        <v>75</v>
+        <v>51</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f>"24"</f>
+        <v>24</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'TDF', 'Tierra del Fuego')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'TDF', 'Tierra del Fuego');</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1555,21 +1511,25 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" t="s">
-        <v>78</v>
+        <v>23</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f>"99"</f>
+        <v>99</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `cod_provincia`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), '1', 'TUC', 'Tucumán')</v>
+        <v>INSERT INTO `sise_legal`.`ref_direccion_provincia` (`usr_ult_modif`, `fec_ult_modif`, `observaciones`, `provincia`) VALUES ('1', SYSDATE(), 'NA', 'Desconocido');</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E26">
+    <sortCondition ref="D2:D26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>